<commit_message>
last version of entrega 3
</commit_message>
<xml_diff>
--- a/Entregables/1. Entrega Informe Inicial/gantt.xlsx
+++ b/Entregables/1. Entrega Informe Inicial/gantt.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Task</t>
   </si>
@@ -89,10 +89,25 @@
     <t>NEW</t>
   </si>
   <si>
-    <t>Reschedule Days</t>
+    <t>Reschedule Days 1</t>
   </si>
   <si>
-    <t>start reschedule</t>
+    <t>start reschedule 1</t>
+  </si>
+  <si>
+    <t>Duration 1</t>
+  </si>
+  <si>
+    <t>Reschedule Days 2</t>
+  </si>
+  <si>
+    <t>start reschedule 2</t>
+  </si>
+  <si>
+    <t>Duration 2</t>
+  </si>
+  <si>
+    <t>User testing, general</t>
   </si>
 </sst>
 </file>
@@ -248,7 +263,7 @@
                   <c:v>Neural Network</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>User testing</c:v>
+                  <c:v>User testing, general</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Mock up blur</c:v>
@@ -487,6 +502,25 @@
             </c:extLst>
           </c:dPt>
           <c:dPt>
+            <c:idx val="7"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000002B-2608-45A1-B5EA-49BC08FAF7C5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
             <c:idx val="8"/>
             <c:invertIfNegative val="0"/>
             <c:bubble3D val="0"/>
@@ -518,6 +552,153 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000F-2608-45A1-B5EA-49BC08FAF7C5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="10"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000047-2608-45A1-B5EA-49BC08FAF7C5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000004D-2608-45A1-B5EA-49BC08FAF7C5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="12"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000050-2608-45A1-B5EA-49BC08FAF7C5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="13"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001F-2608-45A1-B5EA-49BC08FAF7C5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="14"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000056-2608-45A1-B5EA-49BC08FAF7C5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="15"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000001B-2608-45A1-B5EA-49BC08FAF7C5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="16"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000059-2608-45A1-B5EA-49BC08FAF7C5}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:cat>
             <c:strRef>
@@ -552,7 +733,7 @@
                   <c:v>Neural Network</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>User testing</c:v>
+                  <c:v>User testing, general</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Mock up blur</c:v>
@@ -588,7 +769,7 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55</c:v>
+                  <c:v>91</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>19</c:v>
@@ -653,7 +834,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Reschedule Days</c:v>
+                  <c:v>Reschedule Days 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -718,7 +899,7 @@
                   <c:v>Neural Network</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>User testing</c:v>
+                  <c:v>User testing, general</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Mock up blur</c:v>
@@ -754,7 +935,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>69</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -772,7 +953,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>8</c:v>
@@ -781,10 +962,10 @@
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -799,7 +980,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>43</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -819,7 +1000,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Duration</c:v>
+                  <c:v>Duration 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -836,6 +1017,86 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000035-2608-45A1-B5EA-49BC08FAF7C5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="5"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000003C-2608-45A1-B5EA-49BC08FAF7C5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="8"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000042-2608-45A1-B5EA-49BC08FAF7C5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="9"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000064-2608-45A1-B5EA-49BC08FAF7C5}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:cat>
             <c:strRef>
               <c:f>Hoja1!$B$3:$B$19</c:f>
@@ -869,7 +1130,7 @@
                   <c:v>Neural Network</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>User testing</c:v>
+                  <c:v>User testing, general</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>Mock up blur</c:v>
@@ -911,7 +1172,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>10</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6</c:v>
@@ -920,19 +1181,19 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>21</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -947,7 +1208,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -955,6 +1216,184 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{0000004A-B477-4AF3-9ED6-3AF73ADC2D39}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$I$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Reschedule Days 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$I$3:$I$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000003D-2608-45A1-B5EA-49BC08FAF7C5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Hoja1!$K$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Duration 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FFC000"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:val>
+            <c:numRef>
+              <c:f>Hoja1!$K$3:$K$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{0000003E-2608-45A1-B5EA-49BC08FAF7C5}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1674,16 +2113,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>292485</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>61864</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1165611</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>423333</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>74084</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>365125</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>186844</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2008,21 +2447,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:H32"/>
+  <dimension ref="A2:K32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C3" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="T19" sqref="T19"/>
+    <sheetView tabSelected="1" topLeftCell="G19" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="26.140625" customWidth="1"/>
     <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" customWidth="1"/>
     <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="17.5703125" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -2042,10 +2483,19 @@
         <v>22</v>
       </c>
       <c r="H2" t="s">
-        <v>2</v>
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" t="s">
+        <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
         <v>6</v>
       </c>
@@ -2067,8 +2517,16 @@
         <f>IF(F3&lt;&gt;0,D3,)</f>
         <v>0</v>
       </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I19" si="0">IF(ISBLANK(J3),,J3-G3-H3)</f>
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K19" si="1">IF(I3&lt;&gt;0,D3,)</f>
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
@@ -2076,18 +2534,25 @@
         <v>43157</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D19" si="0">E4-C4</f>
-        <v>55</v>
+        <f t="shared" ref="D4:D19" si="2">E4-C4</f>
+        <v>91</v>
       </c>
       <c r="E4" s="1">
-        <v>43212</v>
+        <v>43248</v>
       </c>
       <c r="F4">
-        <f>124-55</f>
-        <v>69</v>
+        <v>33</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B5" s="5" t="s">
         <v>17</v>
       </c>
@@ -2095,22 +2560,30 @@
         <v>43262</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="E5" s="1">
         <v>43281</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F4:F19" si="1">IF(ISBLANK(G5),,G5-E5)</f>
+        <f t="shared" ref="F5:F19" si="3">IF(ISBLANK(G5),,G5-E5)</f>
         <v>0</v>
       </c>
       <c r="H5">
-        <f t="shared" ref="H4:H19" si="2">IF(F5&lt;&gt;0,D5,)</f>
+        <f t="shared" ref="H5:H19" si="4">IF(F5&lt;&gt;0,D5,)</f>
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
@@ -2118,22 +2591,30 @@
         <v>43171</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="E6" s="1">
         <v>43177</v>
       </c>
       <c r="F6">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K6">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H6">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
@@ -2141,25 +2622,34 @@
         <v>43174</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="E7" s="1">
         <v>43184</v>
       </c>
       <c r="F7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>29</v>
       </c>
       <c r="G7" s="1">
         <v>43213</v>
       </c>
       <c r="H7">
-        <f t="shared" si="2"/>
-        <v>10</v>
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="J7" s="1">
+        <v>43248</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
@@ -2167,25 +2657,36 @@
         <v>43185</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="E8" s="1">
         <v>43191</v>
       </c>
       <c r="F8">
-        <f t="shared" si="1"/>
+        <f>IF(ISBLANK(G8),,G8-E8)</f>
         <v>29</v>
       </c>
       <c r="G8" s="1">
         <v>43220</v>
       </c>
       <c r="H8">
-        <f t="shared" si="2"/>
+        <f>IF(F8&lt;&gt;0,D8,)</f>
         <v>6</v>
       </c>
+      <c r="I8">
+        <f>IF(ISBLANK(J8),,J8-G8-H8)</f>
+        <v>22</v>
+      </c>
+      <c r="J8" s="1">
+        <v>43248</v>
+      </c>
+      <c r="K8">
+        <f>IF(I8&lt;&gt;0,D8,)</f>
+        <v>6</v>
+      </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
@@ -2193,22 +2694,30 @@
         <v>43171</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="E9" s="1">
         <v>43184</v>
       </c>
       <c r="F9">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -2219,22 +2728,34 @@
         <v>43213</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="E10" s="1">
         <v>43220</v>
       </c>
       <c r="F10">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="G10" s="1">
+        <v>43248</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="I10">
+        <f>IF(ISBLANK(J10),,J10-G10-H10)</f>
+        <v>0</v>
+      </c>
+      <c r="J10" s="1"/>
+      <c r="K10">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>10</v>
       </c>
@@ -2242,33 +2763,42 @@
         <v>43191</v>
       </c>
       <c r="D11">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="E11" s="1">
+        <v>43212</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="G11" s="1">
+        <v>43220</v>
+      </c>
+      <c r="H11">
+        <v>7</v>
+      </c>
+      <c r="I11">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="E11" s="1">
-        <v>43212</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="G11" s="1">
-        <v>43220</v>
-      </c>
-      <c r="H11">
-        <f t="shared" si="2"/>
-        <v>21</v>
+      <c r="J11" s="1">
+        <v>43248</v>
+      </c>
+      <c r="K11">
+        <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C12" s="1">
         <v>43199</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="E12" s="1">
@@ -2282,80 +2812,121 @@
         <v>43228</v>
       </c>
       <c r="H12">
+        <f>IF(F12&lt;&gt;0,D12,)</f>
+        <v>13</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="J12" s="1">
+        <v>43264</v>
+      </c>
+      <c r="K12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1">
+        <v>43213</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E13" s="1">
+        <v>43215</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="G13" s="1">
+        <v>43262</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="4"/>
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J13" s="1"/>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="1">
+        <v>43213</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E14" s="1">
+        <v>43216</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="G14" s="1">
+        <v>43264</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="4"/>
+        <v>3</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1">
+        <v>43227</v>
+      </c>
+      <c r="D15">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="1">
-        <v>43213</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="E13" s="1">
-        <v>43215</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C14" s="1">
-        <v>43213</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="E14" s="1">
-        <v>43216</v>
-      </c>
-      <c r="F14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15" s="1">
-        <v>43227</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
       <c r="E15" s="1">
         <v>43240</v>
       </c>
       <c r="F15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K15">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>15</v>
       </c>
@@ -2363,22 +2934,30 @@
         <v>43241</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="E16" s="6">
         <v>43254</v>
       </c>
       <c r="F16">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H16">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="5" t="s">
         <v>11</v>
       </c>
@@ -2386,22 +2965,30 @@
         <v>43247</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="E17" s="1">
         <v>43254</v>
       </c>
       <c r="F17">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H17">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>18</v>
       </c>
@@ -2409,22 +2996,30 @@
         <v>43220</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="E18" s="1">
         <v>43226</v>
       </c>
       <c r="F18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H18">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>16</v>
       </c>
@@ -2432,25 +3027,41 @@
         <v>43213</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="E19" s="1">
         <v>43219</v>
       </c>
       <c r="F19">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="G19" s="1">
+        <v>43262</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K19">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
     </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="E31" s="1">
+        <v>43246</v>
+      </c>
+    </row>
+    <row r="32" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E32">
-        <f>C4-F32</f>
-        <v>-124</v>
+        <f>E31-F32</f>
+        <v>-35</v>
       </c>
       <c r="F32" s="1">
         <v>43281</v>

</xml_diff>